<commit_message>
fixed formatting in Main, added process name to Config
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\P3\uipath-automation-6\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cito\Revature\UiPath Project 3\uipath-automation-6\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE31F7E-9E4E-4877-AF6D-4FF088B31EED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014BBFA1-B2EB-4C3F-AE4B-A17BB6E6D21B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2004" yWindow="756" windowWidth="17280" windowHeight="8976" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -87,9 +87,6 @@
     <t>logF_BusinessProcessName</t>
   </si>
   <si>
-    <t>Framework</t>
-  </si>
-  <si>
     <t>ProcessABCQueue</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -170,6 +167,9 @@
   </si>
   <si>
     <t>Message to write to transaction item Status column if transaction is/was pending processing.</t>
+  </si>
+  <si>
+    <t>CreateGitHubOrganization</t>
   </si>
 </sst>
 </file>
@@ -547,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -595,13 +595,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -610,42 +610,42 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
         <v>39</v>
       </c>
-      <c r="B7" t="s">
-        <v>40</v>
-      </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
         <v>43</v>
-      </c>
-      <c r="B9" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1647,7 +1647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1701,7 +1701,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1725,7 +1725,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -1747,7 +1747,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -1758,7 +1758,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1769,41 +1769,41 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
         <v>31</v>
       </c>
-      <c r="B12" t="s">
-        <v>32</v>
-      </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
         <v>45</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>46</v>
-      </c>
-      <c r="C14" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>